<commit_message>
chcked and fixed the ers
</commit_message>
<xml_diff>
--- a/Files/college_info/all_colleges/CBIT/CBIT_placements.xlsx
+++ b/Files/college_info/all_colleges/CBIT/CBIT_placements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammad Arshad Ali\Dropbox\Programming\KMIT\Projects\group\python project on dataset (1st year 2nd sem)\files\CBIT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91703\Desktop\gitt\PYTHON PROJECT\github\python_project-dataset\Files\college_info\all_colleges\CBIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4CCEAB-445D-4EE0-822B-DFA14212BFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007CFBCA-2F39-42EF-9D04-05C444F055AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
   <si>
     <r>
       <rPr>
@@ -1482,6 +1482,145 @@
   </si>
   <si>
     <t>OFFERS</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>Microchip</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial MT"/>
+      </rPr>
+      <t>-2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>Micron</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial MT"/>
+      </rPr>
+      <t>-2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>Model N</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial MT"/>
+      </rPr>
+      <t>-2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>Capgemini (Interim Selects)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial MT"/>
+      </rPr>
+      <t>-2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>Keka Ltd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial MT"/>
+      </rPr>
+      <t>-2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>alliantgroup</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial MT"/>
+      </rPr>
+      <t>-2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>HCL Technologies Ltd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial MT"/>
+      </rPr>
+      <t>-2</t>
+    </r>
+  </si>
+  <si>
+    <t>Keka Ltd-3</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>Alliant Group</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial MT"/>
+      </rPr>
+      <t>-2</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1555,7 +1694,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1598,11 +1737,45 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1939,7 +2112,7 @@
   <dimension ref="A1:E158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -2359,8 +2532,8 @@
       <c r="A28" s="3">
         <v>27</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>57</v>
+      <c r="B28" s="14" t="s">
+        <v>149</v>
       </c>
       <c r="C28" s="3">
         <v>11</v>
@@ -2569,8 +2742,8 @@
       <c r="A42" s="3">
         <v>41</v>
       </c>
-      <c r="B42" s="4" t="s">
-        <v>10</v>
+      <c r="B42" s="14" t="s">
+        <v>150</v>
       </c>
       <c r="C42" s="5">
         <v>8.1</v>
@@ -2659,8 +2832,8 @@
       <c r="A48" s="3">
         <v>47</v>
       </c>
-      <c r="B48" s="4" t="s">
-        <v>72</v>
+      <c r="B48" s="14" t="s">
+        <v>151</v>
       </c>
       <c r="C48" s="10">
         <v>7.61</v>
@@ -2719,8 +2892,8 @@
       <c r="A52" s="3">
         <v>51</v>
       </c>
-      <c r="B52" s="4" t="s">
-        <v>22</v>
+      <c r="B52" s="14" t="s">
+        <v>152</v>
       </c>
       <c r="C52" s="5">
         <v>7.5</v>
@@ -2824,8 +2997,8 @@
       <c r="A59" s="3">
         <v>58</v>
       </c>
-      <c r="B59" s="4" t="s">
-        <v>41</v>
+      <c r="B59" s="14" t="s">
+        <v>153</v>
       </c>
       <c r="C59" s="5">
         <v>7</v>
@@ -2974,8 +3147,8 @@
       <c r="A69" s="3">
         <v>68</v>
       </c>
-      <c r="B69" s="4" t="s">
-        <v>51</v>
+      <c r="B69" s="14" t="s">
+        <v>154</v>
       </c>
       <c r="C69" s="5">
         <v>6.5</v>
@@ -3079,8 +3252,8 @@
       <c r="A76" s="3">
         <v>75</v>
       </c>
-      <c r="B76" s="4" t="s">
-        <v>43</v>
+      <c r="B76" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="C76" s="5">
         <v>6</v>
@@ -3844,8 +4017,8 @@
       <c r="A127" s="11">
         <v>126</v>
       </c>
-      <c r="B127" s="4" t="s">
-        <v>41</v>
+      <c r="B127" s="14" t="s">
+        <v>156</v>
       </c>
       <c r="C127" s="5">
         <v>4</v>
@@ -3919,8 +4092,8 @@
       <c r="A132" s="11">
         <v>131</v>
       </c>
-      <c r="B132" s="4" t="s">
-        <v>108</v>
+      <c r="B132" s="14" t="s">
+        <v>157</v>
       </c>
       <c r="C132" s="5">
         <v>4</v>
@@ -4300,6 +4473,10 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A161">
     <sortCondition ref="A1:A161"/>
   </sortState>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>